<commit_message>
filled in most of the entries for Tahoe-LAFS
</commit_message>
<xml_diff>
--- a/Systems-Comparison.xlsx
+++ b/Systems-Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sic2/git/sos-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA02212-761C-4643-A169-BA47229033D9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B01B73-8C3D-1B48-98B3-35D10A6929A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="34120" windowHeight="31560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="31560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qualitative evaluation" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="254">
   <si>
     <t>Other</t>
   </si>
@@ -531,12 +531,6 @@
     <t>deltas (neighbour deltas are merged from time to time to avoid too many deltas being applied)</t>
   </si>
   <si>
-    <t>PAST</t>
-  </si>
-  <si>
-    <t>DHT - Pastry</t>
-  </si>
-  <si>
     <t>Y (committed/authort)</t>
   </si>
   <si>
@@ -681,9 +675,6 @@
     <t>in transit</t>
   </si>
   <si>
-    <t>Y - at rest</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
@@ -700,6 +691,102 @@
   </si>
   <si>
     <t>in transit and at rest (mix of RSA and AES encryption)</t>
+  </si>
+  <si>
+    <t>FARSITE</t>
+  </si>
+  <si>
+    <t>CFS</t>
+  </si>
+  <si>
+    <t>Chord File System</t>
+  </si>
+  <si>
+    <t>partially decentralised</t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>DHash DHT</t>
+  </si>
+  <si>
+    <t>DHash DHT - Chord</t>
+  </si>
+  <si>
+    <t>distributed - Pastry overlay network</t>
+  </si>
+  <si>
+    <t>DHT - PAST</t>
+  </si>
+  <si>
+    <t>Pastis</t>
+  </si>
+  <si>
+    <t>PhD thesis titled "Self-certifying file system"</t>
+  </si>
+  <si>
+    <t>Internals location</t>
+  </si>
+  <si>
+    <t>.git/</t>
+  </si>
+  <si>
+    <t>~/.tahoe/</t>
+  </si>
+  <si>
+    <t>.hg/</t>
+  </si>
+  <si>
+    <t>~/.ipfs/</t>
+  </si>
+  <si>
+    <t>check paths from configuration files found here: ~./config/camlistore/</t>
+  </si>
+  <si>
+    <t>~/sos/ (or based on configuration)</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>Y - at rest - file is encrypted first and then chunked into small segments</t>
+  </si>
+  <si>
+    <t>Y (only 3 blocks out of 10 are needed to recontruct a segment with the default settings)</t>
+  </si>
+  <si>
+    <t>Y - with Merkle Trees</t>
+  </si>
+  <si>
+    <t>REST, FTP, SFTP</t>
+  </si>
+  <si>
+    <t>represented as the edges of the graph</t>
+  </si>
+  <si>
+    <t>internal nodes in the graph</t>
+  </si>
+  <si>
+    <t>after file has been encrypted - called "share" (for the key-value store) - by default there are 10 shares per file - or segments</t>
+  </si>
+  <si>
+    <t>Simple Secure Storage Service (S4)</t>
+  </si>
+  <si>
+    <t>https://leastauthority.com/</t>
+  </si>
+  <si>
+    <t>See Tahoe-LAFS</t>
+  </si>
+  <si>
+    <t>Commercial product built on top of Tahoe-LAFS</t>
+  </si>
+  <si>
+    <t>SHA-256d (called capabilities)</t>
+  </si>
+  <si>
+    <t>Y --&gt; three types: normal (for immutable file) and read-only and read-write (for mutable file)</t>
   </si>
 </sst>
 </file>
@@ -730,7 +817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,6 +833,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,6 +951,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -867,10 +963,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1153,13 +1246,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C67EC2-0C6F-4549-A1AC-EB375A4E7ABD}">
-  <dimension ref="A1:AW56"/>
+  <dimension ref="A1:BD57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z37" sqref="Z37"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,110 +1265,119 @@
     <col min="6" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="23" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1"/>
-    <col min="11" max="11" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="52.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="10.83203125" style="1"/>
-    <col min="19" max="19" width="55.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" style="1" customWidth="1"/>
-    <col min="24" max="24" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="38.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.83203125" style="1"/>
-    <col min="28" max="28" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.83203125" style="1"/>
-    <col min="30" max="30" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="10.83203125" style="1"/>
-    <col min="36" max="36" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="13.6640625" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="11" width="10.83203125" style="1"/>
+    <col min="12" max="16" width="10.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="52.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="10.83203125" style="1"/>
+    <col min="25" max="25" width="55.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21" style="1" customWidth="1"/>
+    <col min="30" max="30" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.6640625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="38.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="38.5" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" style="1"/>
+    <col min="35" max="35" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.83203125" style="1"/>
+    <col min="37" max="37" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="42" width="10.83203125" style="1"/>
+    <col min="43" max="43" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="13.6640625" style="1" customWidth="1"/>
+    <col min="46" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="3" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" s="3" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="C1" s="10"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="14" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="15"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="14" t="s">
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="14" t="s">
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="18" t="s">
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="14" t="s">
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="3" t="s">
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AM1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="14" t="s">
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="14" t="s">
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="14" t="s">
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="14" t="s">
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="3" t="s">
+      <c r="AZ1" s="16"/>
+      <c r="BA1" s="16"/>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -1300,127 +1402,142 @@
         <v>152</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="K2" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT2" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1436,32 +1553,20 @@
       <c r="H3" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
+      <c r="Q3" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>27</v>
@@ -1469,44 +1574,59 @@
       <c r="Y3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="AA3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>27</v>
+        <v>207</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AO3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
@@ -1516,38 +1636,41 @@
       <c r="E4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="S4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="X4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Z4" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AF4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
@@ -1560,87 +1683,99 @@
       <c r="E5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="S5" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF5" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AG5" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="X6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Z6" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AF6" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:56" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Z8" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AF8" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="C9" s="11"/>
     </row>
-    <row r="10" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:56" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
@@ -1663,31 +1798,37 @@
         <v>84</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="AD10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="AE10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AU10" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AV10" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:49" ht="64" x14ac:dyDescent="0.2">
+      <c r="BB10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BC10" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>43</v>
       </c>
@@ -1701,22 +1842,28 @@
         <v>156</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="K11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="X11" s="1" t="s">
+      <c r="T11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AD11" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:56" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>134</v>
       </c>
@@ -1732,17 +1879,17 @@
       <c r="H12" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="S12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
@@ -1752,26 +1899,26 @@
       <c r="D13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>215</v>
+      <c r="Q13" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="Z13" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AF13" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>108</v>
       </c>
@@ -1787,35 +1934,35 @@
       <c r="J14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="N14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AF14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AM14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
@@ -1825,14 +1972,17 @@
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="Q15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>79</v>
       </c>
@@ -1843,13 +1993,19 @@
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="M16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="T16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
@@ -1859,20 +2015,20 @@
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:49" ht="64" x14ac:dyDescent="0.2">
+      <c r="Q17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:56" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>95</v>
       </c>
@@ -1894,20 +2050,23 @@
       <c r="H18" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AU18" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="R18" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="BB18" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>107</v>
       </c>
@@ -1923,20 +2082,23 @@
       <c r="J19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="L19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+      <c r="Q19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:56" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>123</v>
       </c>
@@ -1958,20 +2120,20 @@
       <c r="H20" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+      <c r="S20" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
@@ -1991,7 +2153,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>161</v>
       </c>
@@ -2011,20 +2173,20 @@
         <v>137</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="K22" s="12" t="s">
+      <c r="Q22" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="R22" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="N22" s="12" t="s">
+      <c r="T22" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="P22" s="12" t="s">
+      <c r="V22" s="12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>104</v>
       </c>
@@ -2034,17 +2196,20 @@
       <c r="D23" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="24" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+      <c r="S23" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>160</v>
       </c>
@@ -2069,32 +2234,14 @@
       <c r="I24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="Q24" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>27</v>
+        <v>202</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>29</v>
@@ -2103,15 +2250,18 @@
         <v>29</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AA24" s="1" t="s">
@@ -2129,12 +2279,6 @@
       <c r="AE24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG24" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="AH24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2144,6 +2288,15 @@
       <c r="AJ24" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AK24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM24" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="AN24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2156,15 +2309,6 @@
       <c r="AQ24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AR24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT24" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="AU24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2174,45 +2318,72 @@
       <c r="AW24" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AX24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AZ24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="T25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+      <c r="R26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>45</v>
       </c>
@@ -2222,11 +2393,14 @@
       <c r="D27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="S27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>46</v>
       </c>
@@ -2245,56 +2419,56 @@
       <c r="G28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AO28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AP28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AQ28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT28" s="1" t="s">
+      <c r="AU28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AW28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:49" ht="48" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="AX28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AZ28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:56" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>80</v>
       </c>
@@ -2313,15 +2487,15 @@
       <c r="G29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="C30" s="11"/>
     </row>
-    <row r="31" spans="1:49" ht="64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:56" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>99</v>
       </c>
@@ -2329,7 +2503,7 @@
         <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>102</v>
@@ -2340,70 +2514,76 @@
       <c r="G31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Z31" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="S31" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC32" s="1" t="s">
+      <c r="S32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AI32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP32" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>47</v>
       </c>
@@ -2411,28 +2591,28 @@
         <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="N35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="T35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AA35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD35" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+      <c r="AH35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK35" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>138</v>
       </c>
@@ -2451,25 +2631,25 @@
       <c r="G36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="X36" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="Z36" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AF36" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
@@ -2486,184 +2666,209 @@
       <c r="G37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="T37" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:56" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:49" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:56" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="C40" s="11"/>
     </row>
-    <row r="41" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:56" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU41" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AV41" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="1:49" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S41" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BB41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BC41" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:56" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN43" s="1" t="s">
+      <c r="S43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU43" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AP43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ43" s="1" t="s">
+      <c r="AW43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AR43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AU43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AW43" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="AY43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AZ43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD43" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AN44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AO44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AR44" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS44" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT44" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="AU44" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AV44" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AW44" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="AX44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AZ44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BD44" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AQ46" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:49" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AX46" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:56" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
       <c r="C47" s="11"/>
     </row>
-    <row r="51" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="C51" s="11"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:20" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q52" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="R52" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="T52" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+    <row r="54" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+      <c r="S54" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
+    <row r="56" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="6"/>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="P1:S1"/>
+  <mergeCells count="12">
+    <mergeCell ref="V1:Y1"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="AR1:AT1"/>
+    <mergeCell ref="AP1:AQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>